<commit_message>
Update readme and code
</commit_message>
<xml_diff>
--- a/build/classes/ql_phan_thuong/excel/KhenThuongCuoiNam.xlsx
+++ b/build/classes/ql_phan_thuong/excel/KhenThuongCuoiNam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PV\Documents\NetBeansProjects\QL_Phan_Thuong\src\ql_phan_thuong\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TaHa\Desktop\BTL\NMCNPM_Nhom5\src\ql_phan_thuong\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C6AB62-44A3-40BB-A1A4-1F2D1CE1DB15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7EA1D6-EF57-48FB-95F5-ECE38824D1CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{433B8C56-DF23-45B9-A969-35C3CBA84002}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{433B8C56-DF23-45B9-A969-35C3CBA84002}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -33,60 +33,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
-  <si>
-    <t>Nguyễn Bá Đức</t>
-  </si>
-  <si>
-    <t>Nguyễn Bá Chiến</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Bình</t>
-  </si>
-  <si>
-    <t>Lớp KHMT 01 K63 HUST</t>
-  </si>
-  <si>
-    <t>Học Sinh ProVip</t>
-  </si>
-  <si>
-    <t>Maybach S650</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>src/ql_phan_thuong/Picture/aaimage.jpg</t>
-  </si>
-  <si>
-    <t>src/ql_phan_thuong/Picture/cheamsponk.png</t>
-  </si>
-  <si>
-    <t>aaaa</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Hust</t>
-  </si>
-  <si>
-    <t>Đẹp Trai</t>
-  </si>
-  <si>
-    <t>src/ql_phan_thuong/Picture/Nguyễn Bá ĐứcAimage.jpg</t>
-  </si>
-  <si>
-    <t>b</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>Đinh Thu Thắm</t>
+  </si>
+  <si>
+    <t>Đinh Nguyễn Hoàng Anh</t>
+  </si>
+  <si>
+    <t>Lê Thị Thu</t>
+  </si>
+  <si>
+    <t>TH MK</t>
+  </si>
+  <si>
+    <t>Học sinh giỏi</t>
+  </si>
+  <si>
+    <t>src/ql_phan_thuong/Picture/Đinh Thu Thắm_Đinh Nguyễn Hoàng Anh_Lê Thị Thuimage.jpg</t>
+  </si>
+  <si>
+    <t>Sách</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>Họ tên</t>
+  </si>
+  <si>
+    <t>Họ tên bố</t>
+  </si>
+  <si>
+    <t>Họ tên mẹ</t>
+  </si>
+  <si>
+    <t>Trường</t>
+  </si>
+  <si>
+    <t>Thành tích</t>
+  </si>
+  <si>
+    <t>Quà tặng</t>
+  </si>
+  <si>
+    <t>Giá trị</t>
+  </si>
+  <si>
+    <t>Minh chứng</t>
+  </si>
+  <si>
+    <t>Đinh Thu Hà</t>
+  </si>
+  <si>
+    <t>src/ql_phan_thuong/Picture/Đinh Thu Hà_Đinh Nguyễn Hoàng Anh_Lê Thị Thuimage.jpg</t>
+  </si>
+  <si>
+    <t>Năm</t>
   </si>
 </sst>
 </file>
@@ -438,197 +444,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2D67BB-D678-4D44-9729-777A26C3D213}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="79.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="97.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="G2" t="s">
         <v>5</v>
-      </c>
-      <c r="I1">
-        <v>15000000000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="I2">
-        <v>10000</v>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6">
-        <v>11000</v>
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>